<commit_message>
Arreglo de errores en BOM de B y C
</commit_message>
<xml_diff>
--- a/Hardware/Satelite/PCB_B/BOM_B.xlsx
+++ b/Hardware/Satelite/PCB_B/BOM_B.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msys32\home\tmax4\esp\Hardware\Satelite\PCB_B\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{96B8B606-ACB5-4E83-ACE1-8926F12477C9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44361CFA-7C02-4109-B8BA-9BC5CBCB59AD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PCB_B" sheetId="1" r:id="rId1"/>
@@ -388,7 +388,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00000"/>
   </numFmts>
@@ -933,14 +933,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:E36" totalsRowShown="0">
-  <autoFilter ref="A1:E36"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla1" displayName="Tabla1" ref="A1:E36" totalsRowShown="0">
+  <autoFilter ref="A1:E36" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Qty"/>
-    <tableColumn id="2" name="Reference(s)"/>
-    <tableColumn id="3" name="Value"/>
-    <tableColumn id="4" name="Footprint"/>
-    <tableColumn id="5" name="Manufacturer Part Number"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Qty"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Reference(s)"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Value"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Footprint"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Manufacturer Part Number"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1242,12 +1242,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1413,7 +1413,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B10" t="s">
         <v>27</v>

</xml_diff>